<commit_message>
Add and fix some rules
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
   <si>
     <t>成都</t>
   </si>
@@ -204,6 +204,24 @@
     </rPh>
     <rPh sb="12" eb="13">
       <t>テコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>吃</t>
+    <rPh sb="0" eb="1">
+      <t>チー</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>なし</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必須</t>
+    <rPh sb="0" eb="2">
+      <t>ヒッス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -533,13 +551,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.85"/>
@@ -702,7 +720,7 @@
         <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -832,6 +850,9 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
@@ -840,6 +861,17 @@
       </c>
       <c r="J8" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.85">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>